<commit_message>
Update examples and code revision
- Moved ValidateModelTables to Base
Improved cModelData structure and validation logic.
- Added 'fixed' field to table definitions, and improve cModelTables
- Enhanced cResourceData handling,
- Updated error messages for file not found.
- Various bug fixes and improvements to class interfaces and error reporting.
- Updated example models for consistency.
</commit_message>
<xml_diff>
--- a/Examples/H2SO4plant/H2SO4R_model.xlsx
+++ b/Examples/H2SO4plant/H2SO4R_model.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29127"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ctorr\Documents\Proyectos\TaesLab\Examples\H2SO4plant\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A64C91E-A8ED-4213-BF13-EB5442215123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA5768AD-8125-43A6-B2B5-331C0C6E6E3E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1965" yWindow="435" windowWidth="25740" windowHeight="14700" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PhysicalDiagram" sheetId="5" r:id="rId1"/>
@@ -1092,17 +1092,17 @@
   <sheetPr codeName="Hoja4"/>
   <dimension ref="A1:E11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:E1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7.7109375" customWidth="1"/>
-    <col min="2" max="2" width="15" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="13.5703125" customWidth="1"/>
-    <col min="5" max="5" width="44" customWidth="1"/>
+    <col min="2" max="2" width="13" customWidth="1"/>
+    <col min="3" max="3" width="15" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="16.5703125" customWidth="1"/>
     <col min="6" max="6" width="10" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1111,13 +1111,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>1</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>5</v>
@@ -1128,13 +1128,13 @@
         <v>63</v>
       </c>
       <c r="B2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" t="s">
         <v>74</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>36</v>
-      </c>
-      <c r="D2" t="s">
-        <v>8</v>
       </c>
       <c r="E2" t="s">
         <v>53</v>
@@ -1145,13 +1145,13 @@
         <v>64</v>
       </c>
       <c r="B3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
         <v>75</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>37</v>
-      </c>
-      <c r="D3" t="s">
-        <v>8</v>
       </c>
       <c r="E3" t="s">
         <v>54</v>
@@ -1162,13 +1162,13 @@
         <v>65</v>
       </c>
       <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="s">
         <v>83</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>82</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
       </c>
       <c r="E4" t="s">
         <v>55</v>
@@ -1179,13 +1179,13 @@
         <v>66</v>
       </c>
       <c r="B5" t="s">
+        <v>8</v>
+      </c>
+      <c r="C5" t="s">
         <v>38</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
         <v>39</v>
-      </c>
-      <c r="D5" t="s">
-        <v>8</v>
       </c>
       <c r="E5" t="s">
         <v>56</v>
@@ -1196,13 +1196,13 @@
         <v>67</v>
       </c>
       <c r="B6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C6" t="s">
         <v>76</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
         <v>77</v>
-      </c>
-      <c r="D6" t="s">
-        <v>8</v>
       </c>
       <c r="E6" t="s">
         <v>57</v>
@@ -1213,13 +1213,13 @@
         <v>68</v>
       </c>
       <c r="B7" t="s">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
         <v>40</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
         <v>41</v>
-      </c>
-      <c r="D7" t="s">
-        <v>8</v>
       </c>
       <c r="E7" t="s">
         <v>58</v>
@@ -1230,13 +1230,13 @@
         <v>69</v>
       </c>
       <c r="B8" t="s">
+        <v>8</v>
+      </c>
+      <c r="C8" t="s">
         <v>79</v>
       </c>
-      <c r="C8" t="s">
+      <c r="D8" t="s">
         <v>78</v>
-      </c>
-      <c r="D8" t="s">
-        <v>8</v>
       </c>
       <c r="E8" t="s">
         <v>59</v>
@@ -1247,13 +1247,13 @@
         <v>70</v>
       </c>
       <c r="B9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" t="s">
         <v>43</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>86</v>
-      </c>
-      <c r="D9" t="s">
-        <v>8</v>
       </c>
       <c r="E9" t="s">
         <v>60</v>
@@ -1264,13 +1264,13 @@
         <v>71</v>
       </c>
       <c r="B10" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" t="s">
         <v>80</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>50</v>
-      </c>
-      <c r="D10" t="s">
-        <v>9</v>
       </c>
       <c r="E10" t="s">
         <v>61</v>
@@ -1281,13 +1281,13 @@
         <v>72</v>
       </c>
       <c r="B11" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
         <v>84</v>
       </c>
-      <c r="C11" t="s">
+      <c r="D11" t="s">
         <v>52</v>
-      </c>
-      <c r="D11" t="s">
-        <v>9</v>
       </c>
       <c r="E11" t="s">
         <v>62</v>
@@ -1302,7 +1302,7 @@
           <x14:formula1>
             <xm:f>Validate!$B$2:$B$3</xm:f>
           </x14:formula1>
-          <xm:sqref>D2:D11</xm:sqref>
+          <xm:sqref>B2:B11</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1630,7 +1630,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8628EF63-4DF1-4197-9DD5-3D704F114525}">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>

</xml_diff>